<commit_message>
install axios co the gay bug
</commit_message>
<xml_diff>
--- a/src/assets/template/user.xlsx
+++ b/src/assets/template/user.xlsx
@@ -8,29 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4957CB70-73E7-4F7D-BB18-32C3C4C92CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D49B809F-27CA-40E9-9F8E-2947D22FC540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{3C5F79E0-B0F7-474D-9427-A836F2F7676C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E695CD2E-3798-4E04-8C6D-4F26268632FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="export-user (4)" sheetId="1" r:id="rId1"/>
+    <sheet name="export-user (6)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
-  <si>
-    <t>id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+  <si>
+    <t>name</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -40,73 +37,76 @@
     <t>age</t>
   </si>
   <si>
-    <t>updatedAt</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
+    <t>I'm super admin</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>hn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu </t>
+  </si>
+  <si>
+    <t>nhokanhanh@gmail.com</t>
+  </si>
+  <si>
+    <t>pham ghong thai</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>hr@gmail.com</t>
+  </si>
+  <si>
+    <t>42 Phạm Hồng Thái</t>
+  </si>
+  <si>
+    <t>loe vann nguyen</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>41b le van tho</t>
+  </si>
+  <si>
+    <t>sos nu</t>
+  </si>
+  <si>
     <t>sosnu1111@gmail.com</t>
   </si>
   <si>
-    <t>sos nu</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
     <t>ha-noi</t>
   </si>
   <si>
-    <t>2025-04-20T06:31:45.871342Z</t>
-  </si>
-  <si>
-    <t>[object Object]</t>
-  </si>
-  <si>
     <t>sosnu@gmail.com</t>
   </si>
   <si>
-    <t>2025-04-29T06:38:41.226664Z</t>
+    <t>sos nu1</t>
   </si>
   <si>
     <t>sosnu11111111@gmail.com</t>
   </si>
   <si>
-    <t>sos nu1</t>
-  </si>
-  <si>
-    <t>2025-04-29T06:38:41.303834Z</t>
-  </si>
-  <si>
     <t>so11sn112313123u@gmail.com</t>
   </si>
   <si>
-    <t>2025-04-29T06:44:43.067301Z</t>
-  </si>
-  <si>
     <t>sosnu111111231111@gmail.com</t>
   </si>
   <si>
-    <t>2025-04-29T06:44:43.127383Z</t>
-  </si>
-  <si>
     <t>so11sn112312313123u@gmail.com</t>
   </si>
   <si>
-    <t>2025-04-29T06:48:58.999071Z</t>
-  </si>
-  <si>
     <t>sosnu11111111231111@gmail.com</t>
-  </si>
-  <si>
-    <t>2025-04-29T08:38:05.002035Z</t>
   </si>
 </sst>
 </file>
@@ -966,14 +966,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69051CA-AB69-40EC-B756-3E21A411A55B}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CB7848-2D4B-41D2-9F58-16E6D48998AE}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -992,199 +994,225 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
+      <c r="F6">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
+      <c r="E7">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
+      <c r="F7">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>15</v>
+      <c r="F12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>